<commit_message>
zmienione logi po wyzwoleniu kamery
</commit_message>
<xml_diff>
--- a/Excel/bin/Debug/net8.0-windows/perforex.xlsx
+++ b/Excel/bin/Debug/net8.0-windows/perforex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jabil-my.sharepoint.com/personal/konrad_browalski_jabil_com/Documents/Desktop/perforex/perforex/Excel/bin/Debug/net8.0-windows/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2281209\source\repozytoriaGit\perforex\EnerconMountingJednaList-main\Excel\bin\Debug\net8.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{49E0E793-3F80-420D-B2A5-6048069DF5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D52C8C01-DC8A-4D41-A597-79F953F04DF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FFC730-E764-4351-9722-8434CBDFED3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MUD10UC409 - 1069302_5" sheetId="134" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="178">
   <si>
     <t>1</t>
   </si>
@@ -572,6 +572,9 @@
   </si>
   <si>
     <t>6ab1c1b4-7ce5-11f0-b2f3-0242ac120003</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1223,10 +1226,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1527,8 +1526,8 @@
   <sheetPr codeName="Arkusz8"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,7 +1589,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1616,13 +1615,13 @@
         <v>180</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
@@ -2660,7 +2659,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2695,7 +2694,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2730,7 +2729,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2800,7 +2799,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2835,7 +2834,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2905,7 +2904,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2940,7 +2939,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2975,7 +2974,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3010,7 +3009,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3045,7 +3044,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -3115,7 +3114,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -3150,7 +3149,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -3185,7 +3184,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -3255,7 +3254,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -4296,7 +4295,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -5922,7 +5921,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -5957,7 +5956,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -6027,7 +6026,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -6062,7 +6061,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -6097,7 +6096,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -6132,7 +6131,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -6167,7 +6166,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -6202,7 +6201,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -6237,7 +6236,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -6272,7 +6271,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -6307,7 +6306,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -6342,7 +6341,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -6377,7 +6376,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -6412,7 +6411,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -6447,7 +6446,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -6482,7 +6481,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -6517,7 +6516,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -6552,7 +6551,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -6587,7 +6586,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -6622,7 +6621,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -6657,7 +6656,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -6692,7 +6691,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>90</v>
       </c>
@@ -6727,7 +6726,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>91</v>
       </c>
@@ -6762,7 +6761,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
@@ -6797,7 +6796,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>123</v>
       </c>
@@ -6832,7 +6831,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>124</v>
       </c>
@@ -6867,7 +6866,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>125</v>
       </c>
@@ -6902,7 +6901,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>126</v>
       </c>
@@ -6937,7 +6936,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>129</v>
       </c>
@@ -6972,7 +6971,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
@@ -7007,7 +7006,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>131</v>
       </c>
@@ -7042,7 +7041,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>132</v>
       </c>
@@ -7077,7 +7076,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>135</v>
       </c>
@@ -7112,7 +7111,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>136</v>
       </c>
@@ -7147,7 +7146,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>137</v>
       </c>
@@ -7182,7 +7181,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>138</v>
       </c>
@@ -7217,7 +7216,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>142</v>
       </c>
@@ -7252,7 +7251,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>143</v>
       </c>
@@ -7287,7 +7286,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>144</v>
       </c>
@@ -7322,7 +7321,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>145</v>
       </c>
@@ -8639,17 +8638,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2febb5b2-578a-41f8-a487-d0625abfa65e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="21e01d5e-8ae9-4bde-96aa-caff01f4019d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004EDA7DF4C21185458752CCA2067C25DC" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0f3eafcaa446d0f2f8f74b5449c130b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2febb5b2-578a-41f8-a487-d0625abfa65e" xmlns:ns3="21e01d5e-8ae9-4bde-96aa-caff01f4019d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="813182b2c0603d2da0412929026488bc" ns2:_="" ns3:_="">
     <xsd:import namespace="2febb5b2-578a-41f8-a487-d0625abfa65e"/>
@@ -8860,6 +8848,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2febb5b2-578a-41f8-a487-d0625abfa65e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="21e01d5e-8ae9-4bde-96aa-caff01f4019d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8870,23 +8869,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96BD286E-87B2-4C92-81BB-64509A050BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="21e01d5e-8ae9-4bde-96aa-caff01f4019d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2febb5b2-578a-41f8-a487-d0625abfa65e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12DBA8A9-6132-423C-BA96-1D3730C9C7FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8905,6 +8887,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96BD286E-87B2-4C92-81BB-64509A050BE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="21e01d5e-8ae9-4bde-96aa-caff01f4019d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2febb5b2-578a-41f8-a487-d0625abfa65e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1B81EE-545A-4B7A-98DF-F57859A0CB89}">
   <ds:schemaRefs>

</xml_diff>